<commit_message>
Added pdf of the laba
</commit_message>
<xml_diff>
--- a/3_sem/3.2.3/3_2_3 (1).xlsx
+++ b/3_sem/3.2.3/3_2_3 (1).xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="начало" sheetId="1" state="visible" r:id="rId2"/>
@@ -178,13 +178,12 @@
     <numFmt numFmtId="169" formatCode="#,##0.0"/>
     <numFmt numFmtId="170" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
     </font>
     <font>
       <sz val="10"/>
@@ -206,7 +205,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
@@ -221,15 +219,13 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF767171"/>
-      <name val="Calibri"/>
+      <sz val="9"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <charset val="204"/>
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color rgb="FF767171"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -256,23 +252,16 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="padmaa"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="C059"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -522,11 +511,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -538,7 +527,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -586,11 +575,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -692,7 +681,7 @@
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t>R_L (f)</a:t>
+              <a:t>Зависимость R_L (f)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -726,15 +715,87 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="star"/>
+            <c:size val="17"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="4472c4"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:marker>
+              <c:symbol val="star"/>
+              <c:size val="17"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="4472c4"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:marker>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:marker>
+              <c:symbol val="star"/>
+              <c:size val="17"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="4472c4"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:marker>
+          </c:dPt>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Calibri"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator>; </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Calibri"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator>; </c:separator>
+            </c:dLbl>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
@@ -763,38 +824,6 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="percentage"/>
-            <c:noEndCap val="0"/>
-            <c:val val="0.5"/>
-            <c:spPr>
-              <a:ln w="9360">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-            </c:spPr>
-          </c:errBars>
-          <c:errBars>
-            <c:errDir val="x"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="percentage"/>
-            <c:noEndCap val="0"/>
-            <c:val val="7"/>
-            <c:spPr>
-              <a:ln w="9360">
-                <a:solidFill>
-                  <a:srgbClr val="ed7d31">
-                    <a:alpha val="0"/>
-                  </a:srgbClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-            </c:spPr>
-          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>начало!$C$3:$C$9</c:f>
@@ -864,10 +893,11 @@
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
-            <a:ln w="19080">
+            <a:ln w="9000">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
           </c:spPr>
@@ -935,11 +965,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="61064163"/>
-        <c:axId val="66665524"/>
+        <c:axId val="74928688"/>
+        <c:axId val="97203918"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61064163"/>
+        <c:axId val="74928688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="40"/>
@@ -957,6 +987,34 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>f, кГц</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -983,15 +1041,17 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66665524"/>
+        <c:crossAx val="97203918"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="66665524"/>
+        <c:axId val="97203918"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="5"/>
+          <c:max val="5.55"/>
+          <c:min val="5.15"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1005,6 +1065,34 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Активное сопротивление L, Ом</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1031,9 +1119,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61064163"/>
+        <c:crossAx val="74928688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.05"/>
+        <c:minorUnit val="0.05"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1531,11 +1621,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="6459667"/>
-        <c:axId val="59614398"/>
+        <c:axId val="24614144"/>
+        <c:axId val="67810690"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="6459667"/>
+        <c:axId val="24614144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="18"/>
@@ -1588,12 +1678,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59614398"/>
+        <c:crossAx val="67810690"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="59614398"/>
+        <c:axId val="67810690"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1645,7 +1735,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6459667"/>
+        <c:crossAx val="24614144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2239,11 +2329,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="68164892"/>
-        <c:axId val="4697909"/>
+        <c:axId val="76632834"/>
+        <c:axId val="1342003"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="68164892"/>
+        <c:axId val="76632834"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.15"/>
@@ -2297,12 +2387,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4697909"/>
+        <c:crossAx val="1342003"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="4697909"/>
+        <c:axId val="1342003"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2354,7 +2444,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68164892"/>
+        <c:crossAx val="76632834"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2684,11 +2774,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="77559872"/>
-        <c:axId val="85879464"/>
+        <c:axId val="50006836"/>
+        <c:axId val="30466679"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77559872"/>
+        <c:axId val="50006836"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2753,12 +2843,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85879464"/>
+        <c:crossAx val="30466679"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85879464"/>
+        <c:axId val="30466679"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2823,7 +2913,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77559872"/>
+        <c:crossAx val="50006836"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3040,11 +3130,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="46015565"/>
-        <c:axId val="87839794"/>
+        <c:axId val="30326487"/>
+        <c:axId val="74132071"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="46015565"/>
+        <c:axId val="30326487"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3109,12 +3199,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87839794"/>
+        <c:crossAx val="74132071"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87839794"/>
+        <c:axId val="74132071"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3179,7 +3269,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46015565"/>
+        <c:crossAx val="30326487"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3246,10 +3336,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.103280924113589"/>
-          <c:y val="0.109723111965264"/>
-          <c:w val="0.858414888496711"/>
-          <c:h val="0.70560182219375"/>
+          <c:x val="0.103276781775157"/>
+          <c:y val="0.109679715302491"/>
+          <c:w val="0.858380459631813"/>
+          <c:h val="0.705551601423487"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3743,11 +3833,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="13403237"/>
-        <c:axId val="4505684"/>
+        <c:axId val="84476754"/>
+        <c:axId val="67172448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="13403237"/>
+        <c:axId val="84476754"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.1"/>
@@ -3814,14 +3904,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4505684"/>
-        <c:crossesAt val="0"/>
+        <c:crossAx val="67172448"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.005"/>
         <c:minorUnit val="0.005"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="4505684"/>
+        <c:axId val="67172448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3888,8 +3978,8 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13403237"/>
-        <c:crossesAt val="0"/>
+        <c:crossAx val="84476754"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -3907,8 +3997,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.648844858013798"/>
-          <c:y val="0.896220371556694"/>
+          <c:x val="0.648818834476397"/>
+          <c:y val="0.896156583629893"/>
           <c:w val="0.311086154339804"/>
           <c:h val="0.0661968823403801"/>
         </c:manualLayout>
@@ -4514,11 +4604,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="61210569"/>
-        <c:axId val="73285226"/>
+        <c:axId val="22345878"/>
+        <c:axId val="22483337"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61210569"/>
+        <c:axId val="22345878"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.08"/>
@@ -4600,14 +4690,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73285226"/>
+        <c:crossAx val="22483337"/>
         <c:crossesAt val="0.095"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.01"/>
         <c:minorUnit val="0.01"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73285226"/>
+        <c:axId val="22483337"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.18"/>
@@ -4689,8 +4779,8 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61210569"/>
-        <c:crossesAt val="0"/>
+        <c:crossAx val="22345878"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -4706,8 +4796,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.603500631205432"/>
-          <c:y val="0.944435699669448"/>
+          <c:x val="0.603480040941658"/>
+          <c:y val="0.944361375619737"/>
           <c:w val="0.367054488382408"/>
           <c:h val="0.0453329135841335"/>
         </c:manualLayout>
@@ -4764,7 +4854,7 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>466560</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
+      <xdr:rowOff>151920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4772,7 +4862,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="875880" y="3176280"/>
+        <a:off x="875880" y="3004920"/>
         <a:ext cx="4478400" cy="2862000"/>
       </xdr:xfrm>
       <a:graphic>
@@ -4799,7 +4889,7 @@
       <xdr:col>22</xdr:col>
       <xdr:colOff>54360</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>35640</xdr:rowOff>
+      <xdr:rowOff>187920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4807,7 +4897,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="13277520" y="4831560"/>
+        <a:off x="13277520" y="4583880"/>
         <a:ext cx="4986000" cy="3224160"/>
       </xdr:xfrm>
       <a:graphic>
@@ -4828,8 +4918,8 @@
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>281160</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>189000</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>7920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4837,7 +4927,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="15844320" y="316440"/>
+        <a:off x="15844320" y="297360"/>
         <a:ext cx="7468200" cy="4092120"/>
       </xdr:xfrm>
       <a:graphic>
@@ -4852,14 +4942,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>-360</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>186480</xdr:rowOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>53280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>730080</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>25560</xdr:rowOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>54360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4882,14 +4972,14 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>824760</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>-720</xdr:rowOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>56520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>788040</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>38520</xdr:rowOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>57600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4912,14 +5002,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>270360</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>85320</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>123480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>61200</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>161280</xdr:rowOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>37440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4946,15 +5036,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>802800</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:colOff>358560</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>186840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>210600</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>151560</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>586800</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>189000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4962,7 +5052,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2443680" y="4997520"/>
+        <a:off x="1999440" y="5330520"/>
         <a:ext cx="10551240" cy="4574160"/>
       </xdr:xfrm>
       <a:graphic>
@@ -4981,13 +5071,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L22"/>
+  <dimension ref="A2:L22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N23" activeCellId="0" sqref="N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="6.52"/>
@@ -5002,8 +5092,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="8"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -5041,7 +5130,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="n">
         <v>1</v>
       </c>
@@ -5086,7 +5175,7 @@
         <v>5.28040346263683</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="n">
         <v>2</v>
       </c>
@@ -5131,7 +5220,7 @@
         <v>5.3492337748088</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
         <v>3</v>
       </c>
@@ -5176,7 +5265,7 @@
         <v>5.20046260340217</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="n">
         <v>4</v>
       </c>
@@ -5221,7 +5310,7 @@
         <v>5.44593538326686</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="n">
         <v>5</v>
       </c>
@@ -5266,7 +5355,7 @@
         <v>5.42344323396527</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
         <v>6</v>
       </c>
@@ -5311,7 +5400,7 @@
         <v>5.49550876183624</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
         <v>7</v>
       </c>
@@ -5356,7 +5445,7 @@
         <v>5.47032303484188</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="18" t="s">
         <v>12</v>
       </c>
@@ -5381,7 +5470,7 @@
         <v>5.38075860782258</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="18" t="s">
         <v>13</v>
       </c>
@@ -5403,7 +5492,7 @@
         <v>0.0410664366697353</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -5411,7 +5500,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J14" s="3" t="s">
         <v>15</v>
       </c>
@@ -5419,7 +5508,7 @@
         <v>3.91</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J21" s="22"/>
       <c r="K21" s="3" t="n">
         <v>5.4</v>
@@ -5428,7 +5517,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J22" s="22"/>
       <c r="K22" s="3" t="n">
         <v>5.4</v>
@@ -5458,13 +5547,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:AC54"/>
+  <dimension ref="B2:AC54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="O58" activeCellId="0" sqref="O58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="4" width="10.83"/>
@@ -5475,8 +5564,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="2" width="10.83"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="2" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="23" t="s">
         <v>16</v>
       </c>
@@ -5491,7 +5579,7 @@
       <c r="I2" s="23"/>
       <c r="J2" s="23"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="25" t="s">
         <v>18</v>
       </c>
@@ -5518,7 +5606,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="27" t="n">
         <v>19</v>
       </c>
@@ -5559,7 +5647,7 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="27" t="n">
         <v>19.4</v>
       </c>
@@ -5603,7 +5691,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="27" t="n">
         <v>19.8</v>
       </c>
@@ -5638,7 +5726,7 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="27" t="n">
         <v>20.2</v>
       </c>
@@ -5673,7 +5761,7 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="4"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="27" t="n">
         <v>20.6</v>
       </c>
@@ -5718,7 +5806,7 @@
         <v>0.0579999999999999</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="27" t="n">
         <v>21</v>
       </c>
@@ -5769,7 +5857,7 @@
         <v>15.28</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="27" t="n">
         <v>21.4</v>
       </c>
@@ -5804,7 +5892,7 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="4"/>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="27" t="n">
         <v>21.8</v>
       </c>
@@ -5855,7 +5943,7 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="27" t="n">
         <v>22.2</v>
       </c>
@@ -5897,7 +5985,7 @@
         <v>16.9491525423729</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="27" t="n">
         <v>22.6</v>
       </c>
@@ -5932,7 +6020,7 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="27" t="n">
         <v>23</v>
       </c>
@@ -5967,7 +6055,7 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="4"/>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="27" t="n">
         <v>23.4</v>
       </c>
@@ -6002,7 +6090,7 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="27" t="n">
         <v>23.8</v>
       </c>
@@ -6037,7 +6125,7 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="4"/>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="27" t="n">
         <v>24.2</v>
       </c>
@@ -6072,7 +6160,7 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="4"/>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="27" t="n">
         <v>24.6</v>
       </c>
@@ -6089,7 +6177,7 @@
       </c>
       <c r="F18" s="32"/>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="27" t="n">
         <v>25</v>
       </c>
@@ -6106,7 +6194,7 @@
       </c>
       <c r="F19" s="32"/>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="27" t="n">
         <v>25.4</v>
       </c>
@@ -6123,7 +6211,7 @@
       </c>
       <c r="F20" s="32"/>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="27" t="n">
         <v>25.8</v>
       </c>
@@ -6140,7 +6228,7 @@
       </c>
       <c r="F21" s="32"/>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="2" t="s">
         <v>32</v>
       </c>
@@ -6154,7 +6242,7 @@
         <v>21.4</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="2" t="s">
         <v>33</v>
       </c>
@@ -6168,7 +6256,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N45" s="0" t="n">
         <v>0.707</v>
       </c>
@@ -6176,7 +6264,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N46" s="0" t="n">
         <v>0.707</v>
       </c>
@@ -6202,10 +6290,10 @@
         <v>17.5438596491228</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N53" s="34"/>
     </row>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N54" s="34"/>
     </row>
   </sheetData>
@@ -6229,13 +6317,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:T54"/>
+  <dimension ref="B2:T54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O23" activeCellId="0" sqref="O23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="2" width="10.83"/>
@@ -6246,8 +6334,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="4" width="10.83"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="2" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="23" t="s">
         <v>16</v>
       </c>
@@ -6265,7 +6352,7 @@
       <c r="M2" s="23"/>
       <c r="N2" s="23"/>
     </row>
-    <row r="3" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="25" t="s">
         <v>18</v>
       </c>
@@ -6303,7 +6390,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="39" t="n">
         <v>19</v>
       </c>
@@ -6347,7 +6434,7 @@
         <v>0.162157866546459</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="27" t="n">
         <v>19.4</v>
       </c>
@@ -6391,7 +6478,7 @@
         <v>0.156152019637331</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="27" t="n">
         <v>19.8</v>
       </c>
@@ -6435,7 +6522,7 @@
         <v>0.159154943091895</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="27" t="n">
         <v>20.2</v>
       </c>
@@ -6479,7 +6566,7 @@
         <v>0.156034257933231</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="27" t="n">
         <v>20.6</v>
       </c>
@@ -6523,7 +6610,7 @@
         <v>0.146422547644544</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="27" t="n">
         <v>21</v>
       </c>
@@ -6567,7 +6654,7 @@
         <v>0.136418522650196</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="27" t="n">
         <v>21.4</v>
       </c>
@@ -6611,7 +6698,7 @@
         <v>0.119366207318922</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="27" t="n">
         <v>21.8</v>
       </c>
@@ -6655,7 +6742,7 @@
         <v>0.0744980584685468</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="27" t="n">
         <v>22.2</v>
       </c>
@@ -6699,7 +6786,7 @@
         <v>0.0415186808065814</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="27" t="n">
         <v>22.6</v>
       </c>
@@ -6743,7 +6830,7 @@
         <v>0.0415186808065814</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="27" t="n">
         <v>23</v>
       </c>
@@ -6787,7 +6874,7 @@
         <v>0.0565884242104517</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="27" t="n">
         <v>23.4</v>
       </c>
@@ -6831,7 +6918,7 @@
         <v>0.0723431559508615</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="27" t="n">
         <v>23.8</v>
       </c>
@@ -6875,7 +6962,7 @@
         <v>0.0868117871410338</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="27" t="n">
         <v>24.2</v>
       </c>
@@ -6919,7 +7006,7 @@
         <v>0.103635776897048</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="27" t="n">
         <v>24.6</v>
       </c>
@@ -6943,7 +7030,7 @@
       </c>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="27" t="n">
         <v>25</v>
       </c>
@@ -6967,7 +7054,7 @@
       </c>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="27" t="n">
         <v>25.4</v>
       </c>
@@ -6997,7 +7084,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="27" t="n">
         <v>25.8</v>
       </c>
@@ -7027,11 +7114,11 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M22" s="45"/>
       <c r="N22" s="45"/>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I23" s="2" t="s">
         <v>32</v>
       </c>
@@ -7045,7 +7132,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="2" t="s">
         <v>32</v>
       </c>
@@ -7059,7 +7146,7 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="Q30" s="0" t="s">
         <v>41</v>
       </c>
@@ -7071,13 +7158,13 @@
         <v>0.081</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="T31" s="0" t="n">
         <f aca="false">1/T30</f>
         <v>12.3456790123457</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S33" s="0" t="s">
         <v>43</v>
       </c>
@@ -7095,17 +7182,17 @@
         <v>14.0845070422535</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="47" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="Q36" s="0" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E53" s="2" t="n">
         <v>0.78</v>
       </c>
@@ -7116,7 +7203,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="2" t="n">
         <v>1.2</v>
       </c>

</xml_diff>